<commit_message>
actualizando y revisando valores de PxQ
</commit_message>
<xml_diff>
--- a/Assets/PxQVariosEscenarios.xlsx
+++ b/Assets/PxQVariosEscenarios.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
   <si>
     <t>Escenario 1</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Cantidad Usuarios</t>
   </si>
   <si>
-    <t>Ganacia</t>
-  </si>
-  <si>
     <t>Mes</t>
   </si>
   <si>
@@ -70,6 +67,12 @@
   </si>
   <si>
     <t>Escenario similar a Foursquare (expansión global de aplicación exitosa similar)</t>
+  </si>
+  <si>
+    <t>Ganacia sin costo descarga</t>
+  </si>
+  <si>
+    <t>Ganacia con costo descarga</t>
   </si>
 </sst>
 </file>
@@ -138,184 +141,204 @@
   <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.25887729658792652"/>
-          <c:y val="2.8252405949256341E-2"/>
-          <c:w val="0.65971937882764653"/>
-          <c:h val="0.8326195683872849"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="2"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ganacia sin costo descarga</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$15:$A$38</c:f>
+              <c:f>Sheet1!$C$15:$C$38</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>3.6399999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>18.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>36.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>145.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>364</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>618.79999999999995</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>1092</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8</c:v>
+                  <c:v>1820</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9</c:v>
+                  <c:v>2548</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10</c:v>
+                  <c:v>3567.2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11</c:v>
+                  <c:v>4280.6399999999994</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12</c:v>
+                  <c:v>4708.7039999999997</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>13</c:v>
+                  <c:v>4755.7910400000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>14</c:v>
+                  <c:v>4803.3489504000008</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>15</c:v>
+                  <c:v>4827.3656951520006</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>16</c:v>
+                  <c:v>5020.4603229580798</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>17</c:v>
+                  <c:v>5171.0741326468233</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>18</c:v>
+                  <c:v>5274.4956152997593</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>19</c:v>
+                  <c:v>5432.7304837587526</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>20</c:v>
+                  <c:v>5337.7175422771188</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>21</c:v>
+                  <c:v>5560.1224398719996</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>22</c:v>
+                  <c:v>5673.5943263999989</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>23</c:v>
+                  <c:v>5759.99424</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>24</c:v>
+                  <c:v>5818.1759999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ganacia con costo descarga</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$15:$B$38</c:f>
+              <c:f>Sheet1!$D$15:$D$38</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>150</c:v>
+                  <c:v>61.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>500</c:v>
+                  <c:v>92.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1000</c:v>
+                  <c:v>471.2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3000</c:v>
+                  <c:v>928</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30000</c:v>
+                  <c:v>1427.6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30000</c:v>
+                  <c:v>2584</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>30000</c:v>
+                  <c:v>4140</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>70000</c:v>
+                  <c:v>4996</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>98000</c:v>
+                  <c:v>6994.4</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>117600</c:v>
+                  <c:v>6993.28</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>129360.00000000001</c:v>
+                  <c:v>6712.608000000002</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>130653.60000000002</c:v>
+                  <c:v>5721.3340800000005</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>131960.13600000003</c:v>
+                  <c:v>5778.5474208000023</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>132619.93668000001</c:v>
+                  <c:v>5742.1133579039997</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>137924.73414720001</c:v>
+                  <c:v>6433.6583682201599</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>142062.47617161603</c:v>
+                  <c:v>6494.0481825867673</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>144903.72569504834</c:v>
+                  <c:v>6486.0044120913008</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>149250.83746589979</c:v>
+                  <c:v>6822.6470206256563</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>146640.59182079998</c:v>
+                  <c:v>6015.1927654202582</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>152750.61648</c:v>
+                  <c:v>7148.7288512640025</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>155867.976</c:v>
+                  <c:v>6982.8853247999987</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>158241.60000000001</c:v>
+                  <c:v>7010.1028800000022</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>159840</c:v>
+                  <c:v>7000.9919999999993</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -332,21 +355,20 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="35525376"/>
-        <c:axId val="35526912"/>
+        <c:axId val="100814208"/>
+        <c:axId val="100852864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="35525376"/>
+        <c:axId val="100814208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="35526912"/>
+        <c:crossAx val="100852864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -354,18 +376,18 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="35526912"/>
+        <c:axId val="100852864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="35525376"/>
+        <c:crossAx val="100814208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -403,103 +425,204 @@
   <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.25887729658792652"/>
-          <c:y val="2.8252405949256341E-2"/>
-          <c:w val="0.65971937882764653"/>
-          <c:h val="0.8326195683872849"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$C$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ganacia sin costo descarga</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$B$15:$B$38</c:f>
+              <c:f>Sheet2!$C$15:$C$38</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>20000</c:v>
+                  <c:v>728</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29411.764705882353</c:v>
+                  <c:v>1070.5882352941176</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44117.647058823532</c:v>
+                  <c:v>1605.8823529411766</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>58823.529411764706</c:v>
+                  <c:v>2141.1764705882351</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>88235.294117647063</c:v>
+                  <c:v>3211.7647058823532</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>111764.70588235294</c:v>
+                  <c:v>4068.2352941176464</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>141176.4705882353</c:v>
+                  <c:v>5138.823529411764</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>176470.58823529413</c:v>
+                  <c:v>6423.5294117647063</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>205882.35294117648</c:v>
+                  <c:v>7494.1176470588225</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>235294.11764705883</c:v>
+                  <c:v>8564.7058823529405</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>500000</c:v>
-                </c:pt>
-                <c:pt idx="11" formatCode="General">
-                  <c:v>750000</c:v>
-                </c:pt>
-                <c:pt idx="12" formatCode="General">
-                  <c:v>1000000</c:v>
-                </c:pt>
-                <c:pt idx="13" formatCode="General">
-                  <c:v>1500000</c:v>
-                </c:pt>
-                <c:pt idx="14" formatCode="General">
-                  <c:v>1900000</c:v>
-                </c:pt>
-                <c:pt idx="15" formatCode="General">
-                  <c:v>2400000</c:v>
-                </c:pt>
-                <c:pt idx="16" formatCode="General">
-                  <c:v>3000000</c:v>
-                </c:pt>
-                <c:pt idx="17" formatCode="General">
-                  <c:v>3500000</c:v>
-                </c:pt>
-                <c:pt idx="18" formatCode="General">
-                  <c:v>4000000</c:v>
-                </c:pt>
-                <c:pt idx="19" formatCode="General">
-                  <c:v>4500000</c:v>
-                </c:pt>
-                <c:pt idx="20" formatCode="General">
-                  <c:v>5250000</c:v>
-                </c:pt>
-                <c:pt idx="21" formatCode="General">
-                  <c:v>6000000</c:v>
-                </c:pt>
-                <c:pt idx="22" formatCode="General">
-                  <c:v>6750000</c:v>
-                </c:pt>
-                <c:pt idx="23" formatCode="General">
-                  <c:v>7500000</c:v>
+                  <c:v>18200</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>27300</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>36400</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>54600</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>69160</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>87360</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>109200</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>127400</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>145600</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>163800</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>191100</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>218400</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>245700</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>273000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$D$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ganacia con costo descarga</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$D$15:$D$38</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>4200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3358.8235294117649</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3988.2352941176468</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5835.2941176470595</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7136.4705882352937</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8983.5294117647063</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11082.352941176472</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11752.941176470587</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13011.764705882353</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>47870.588235294126</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>57100</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>67800</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>114200</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>121320</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>152720</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>188400</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>199800</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>221200</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>242600</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>299700</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>331800</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>363900</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>396000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -516,21 +639,20 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="41885696"/>
-        <c:axId val="41887232"/>
+        <c:axId val="45958272"/>
+        <c:axId val="45959808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="41885696"/>
+        <c:axId val="45958272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41887232"/>
+        <c:crossAx val="45959808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -538,7 +660,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="41887232"/>
+        <c:axId val="45959808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -549,180 +671,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41885696"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="es-AR"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet2!$C$15:$C$38</c:f>
-              <c:numCache>
-                <c:formatCode>0</c:formatCode>
-                <c:ptCount val="24"/>
-                <c:pt idx="0">
-                  <c:v>22160</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>12588.235294117647</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>19470.588235294123</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>21058.823529411762</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>38941.176470588245</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>35599.999999999985</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>44658.823529411791</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>54352.941176470602</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>51647.058823529427</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>54823.529411764699</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>318705.8823529412</c:v>
-                </c:pt>
-                <c:pt idx="11" formatCode="General">
-                  <c:v>331000</c:v>
-                </c:pt>
-                <c:pt idx="12" formatCode="General">
-                  <c:v>358000</c:v>
-                </c:pt>
-                <c:pt idx="13" formatCode="General">
-                  <c:v>662000</c:v>
-                </c:pt>
-                <c:pt idx="14" formatCode="General">
-                  <c:v>605200</c:v>
-                </c:pt>
-                <c:pt idx="15" formatCode="General">
-                  <c:v>759200</c:v>
-                </c:pt>
-                <c:pt idx="16" formatCode="General">
-                  <c:v>924000</c:v>
-                </c:pt>
-                <c:pt idx="17" formatCode="General">
-                  <c:v>878000</c:v>
-                </c:pt>
-                <c:pt idx="18" formatCode="General">
-                  <c:v>932000</c:v>
-                </c:pt>
-                <c:pt idx="19" formatCode="General">
-                  <c:v>986000</c:v>
-                </c:pt>
-                <c:pt idx="20" formatCode="General">
-                  <c:v>1317000</c:v>
-                </c:pt>
-                <c:pt idx="21" formatCode="General">
-                  <c:v>1398000</c:v>
-                </c:pt>
-                <c:pt idx="22" formatCode="General">
-                  <c:v>1479000</c:v>
-                </c:pt>
-                <c:pt idx="23" formatCode="General">
-                  <c:v>1560000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="80333056"/>
-        <c:axId val="80334848"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="80333056"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80334848"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="80334848"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="0" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80333056"/>
+        <c:crossAx val="45958272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -749,19 +698,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -784,22 +733,20 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>138112</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -808,36 +755,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1136,14 +1053,15 @@
   <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="D1:K1"/>
+      <selection activeCell="B11" sqref="A3:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
@@ -1191,7 +1109,7 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>1E-3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1199,7 +1117,7 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1207,13 +1125,13 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>0.01</v>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8">
         <v>0.1</v>
@@ -1225,7 +1143,7 @@
       </c>
       <c r="B9">
         <f>B3*B4*4</f>
-        <v>639.36</v>
+        <v>63936</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1233,13 +1151,13 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <f>B3*B5*B6*4</f>
-        <v>639.36</v>
+        <f>B3*B5*B6*4*4</f>
+        <v>5754.24</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <f>B3*B8</f>
@@ -1248,430 +1166,538 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="D14" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
         <v>100</v>
       </c>
-      <c r="C15">
-        <f>B15*4*(B$4+B$5*B$6)+B15*B$8+B15</f>
-        <v>110.8</v>
+      <c r="C15" s="1">
+        <f>(B15*4/1000)*B$4+B15*B$5*B$6*16</f>
+        <v>3.6399999999999997</v>
+      </c>
+      <c r="D15" s="1">
+        <v>4</v>
+      </c>
+      <c r="G15">
+        <f>30000/6</f>
+        <v>5000</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
-      <c r="B16">
-        <v>150</v>
-      </c>
-      <c r="C16">
-        <f>B16*4*(B$4+B$5*B$6)+B16*B$8+B16-B15</f>
-        <v>66.199999999999989</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="1">
+        <v>500</v>
+      </c>
+      <c r="C16" s="1">
+        <f t="shared" ref="C16:C38" si="0">(B16*4/1000)*B$4+B16*B$5*B$6*16</f>
+        <v>18.2</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" ref="D15:D17" si="1">(B16*4/1000)*B$4+B16*B$5*B$6*16*(0.9)+((B16-B15)+B$8*B16)*0.1</f>
+        <v>61.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3</v>
       </c>
-      <c r="B17">
-        <v>500</v>
-      </c>
-      <c r="C17">
-        <f t="shared" ref="C17:C38" si="0">B17*4*(B$4+B$5*B$6)+B17*B$8+B17-B16</f>
-        <v>404</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C17" s="1">
+        <f t="shared" si="0"/>
+        <v>36.4</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="1"/>
+        <v>92.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>4</v>
       </c>
-      <c r="B18">
-        <v>1000</v>
-      </c>
-      <c r="C18">
-        <f t="shared" si="0"/>
-        <v>608</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="1">
+        <v>4000</v>
+      </c>
+      <c r="C18" s="1">
+        <f t="shared" si="0"/>
+        <v>145.6</v>
+      </c>
+      <c r="D18" s="1">
+        <f>(B18*4/1000)*B$4+B18*B$5*B$6*16*(0.9)+((B18-B17)+B$8*B18)*0.1</f>
+        <v>471.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>5</v>
       </c>
-      <c r="B19">
-        <v>3000</v>
-      </c>
-      <c r="C19">
-        <f t="shared" si="0"/>
-        <v>2324</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="1">
+        <v>10000</v>
+      </c>
+      <c r="C19" s="1">
+        <f t="shared" si="0"/>
+        <v>364</v>
+      </c>
+      <c r="D19" s="1">
+        <f>(B19*4/1000)*B$4+B19*B$5*B$6*16*(0.9)+((B19-B18))*0.1</f>
+        <v>928</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>6</v>
       </c>
-      <c r="B20">
-        <v>30000</v>
-      </c>
-      <c r="C20">
-        <f t="shared" si="0"/>
-        <v>30240</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="1">
+        <v>17000</v>
+      </c>
+      <c r="C20" s="1">
+        <f t="shared" si="0"/>
+        <v>618.79999999999995</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" ref="D20:D38" si="2">(B20*4/1000)*B$4+B20*B$5*B$6*16*(0.9)+((B20-B19)+B$8*B20)*0.1</f>
+        <v>1427.6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>7</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="1">
         <v>30000</v>
       </c>
-      <c r="C21">
-        <f t="shared" si="0"/>
-        <v>3240</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="1">
+        <f t="shared" si="0"/>
+        <v>1092</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="2"/>
+        <v>2584</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>8</v>
       </c>
-      <c r="B22">
-        <v>30000</v>
-      </c>
-      <c r="C22">
-        <f t="shared" si="0"/>
-        <v>3240</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="1">
+        <v>50000</v>
+      </c>
+      <c r="C22" s="1">
+        <f t="shared" si="0"/>
+        <v>1820</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="2"/>
+        <v>4140</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>9</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="1">
         <v>70000</v>
       </c>
-      <c r="C23">
-        <f t="shared" si="0"/>
-        <v>47560</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C23" s="1">
+        <f t="shared" si="0"/>
+        <v>2548</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="shared" si="2"/>
+        <v>4996</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>10</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="1">
         <f>B23*1.4</f>
         <v>98000</v>
       </c>
-      <c r="C24">
-        <f t="shared" si="0"/>
-        <v>38584</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C24" s="1">
+        <f t="shared" si="0"/>
+        <v>3567.2</v>
+      </c>
+      <c r="D24" s="1">
+        <f t="shared" si="2"/>
+        <v>6994.4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>11</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="1">
         <f>B24*1.2</f>
         <v>117600</v>
       </c>
-      <c r="C25">
-        <f t="shared" si="0"/>
-        <v>32300.800000000003</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C25" s="1">
+        <f t="shared" si="0"/>
+        <v>4280.6399999999994</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" si="2"/>
+        <v>6993.28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>12</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="1">
         <f>B25*1.1</f>
         <v>129360.00000000001</v>
       </c>
-      <c r="C26">
-        <f t="shared" si="0"/>
-        <v>25730.880000000005</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C26" s="1">
+        <f t="shared" si="0"/>
+        <v>4708.7039999999997</v>
+      </c>
+      <c r="D26" s="1">
+        <f t="shared" si="2"/>
+        <v>6712.608000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>13</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="1">
         <f>B26*1.01</f>
         <v>130653.60000000002</v>
       </c>
-      <c r="C27">
-        <f t="shared" si="0"/>
-        <v>15404.188800000018</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C27" s="1">
+        <f t="shared" si="0"/>
+        <v>4755.7910400000001</v>
+      </c>
+      <c r="D27" s="1">
+        <f t="shared" si="2"/>
+        <v>5721.3340800000005</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>14</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="1">
         <f>B27*1.01</f>
         <v>131960.13600000003</v>
       </c>
-      <c r="C28">
-        <f t="shared" si="0"/>
-        <v>15558.230687999996</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="1">
+        <f t="shared" si="0"/>
+        <v>4803.3489504000008</v>
+      </c>
+      <c r="D28" s="1">
+        <f t="shared" si="2"/>
+        <v>5778.5474208000023</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>15</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="1">
         <f>B28*1.005</f>
         <v>132619.93668000001</v>
       </c>
-      <c r="C29">
-        <f t="shared" si="0"/>
-        <v>14982.75384143999</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C29" s="1">
+        <f t="shared" si="0"/>
+        <v>4827.3656951520006</v>
+      </c>
+      <c r="D29" s="1">
+        <f t="shared" si="2"/>
+        <v>5742.1133579039997</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>16</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="1">
         <f>B29*1.04</f>
         <v>137924.73414720001</v>
       </c>
-      <c r="C30">
-        <f t="shared" si="0"/>
-        <v>20200.668755097606</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C30" s="1">
+        <f t="shared" si="0"/>
+        <v>5020.4603229580798</v>
+      </c>
+      <c r="D30" s="1">
+        <f t="shared" si="2"/>
+        <v>6433.6583682201599</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>17</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="1">
         <f>B30*1.03</f>
         <v>142062.47617161603</v>
       </c>
-      <c r="C31">
-        <f t="shared" si="0"/>
-        <v>19480.489450950554</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C31" s="1">
+        <f t="shared" si="0"/>
+        <v>5171.0741326468233</v>
+      </c>
+      <c r="D31" s="1">
+        <f t="shared" si="2"/>
+        <v>6494.0481825867673</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>18</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="1">
         <f>B31*1.02</f>
         <v>144903.72569504834</v>
       </c>
-      <c r="C32">
-        <f t="shared" si="0"/>
-        <v>18490.851898497524</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C32" s="1">
+        <f t="shared" si="0"/>
+        <v>5274.4956152997593</v>
+      </c>
+      <c r="D32" s="1">
+        <f t="shared" si="2"/>
+        <v>6486.0044120913008</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>19</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="1">
         <f>B32*1.03</f>
         <v>149250.83746589979</v>
       </c>
-      <c r="C33">
-        <f t="shared" si="0"/>
-        <v>20466.20221716864</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C33" s="1">
+        <f t="shared" si="0"/>
+        <v>5432.7304837587526</v>
+      </c>
+      <c r="D33" s="1">
+        <f t="shared" si="2"/>
+        <v>6822.6470206256563</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>20</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="1">
         <f>B35*0.96</f>
         <v>146640.59182079998</v>
       </c>
-      <c r="C34">
-        <f t="shared" si="0"/>
-        <v>13226.938271546591</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C34" s="1">
+        <f t="shared" si="0"/>
+        <v>5337.7175422771188</v>
+      </c>
+      <c r="D34" s="1">
+        <f t="shared" si="2"/>
+        <v>6015.1927654202582</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>21</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="1">
         <f>B36*0.98</f>
         <v>152750.61648</v>
       </c>
-      <c r="C35">
-        <f t="shared" si="0"/>
-        <v>22607.091239040019</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C35" s="1">
+        <f t="shared" si="0"/>
+        <v>5560.1224398719996</v>
+      </c>
+      <c r="D35" s="1">
+        <f t="shared" si="2"/>
+        <v>7148.7288512640025</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>22</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="1">
         <f>B37*0.985</f>
         <v>155867.976</v>
       </c>
-      <c r="C36">
-        <f t="shared" si="0"/>
-        <v>19951.100928</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C36" s="1">
+        <f t="shared" si="0"/>
+        <v>5673.5943263999989</v>
+      </c>
+      <c r="D36" s="1">
+        <f t="shared" si="2"/>
+        <v>6982.8853247999987</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>23</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="1">
         <f>B38*0.99</f>
         <v>158241.60000000001</v>
       </c>
-      <c r="C37">
-        <f t="shared" si="0"/>
-        <v>19463.716800000024</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C37" s="1">
+        <f t="shared" si="0"/>
+        <v>5759.99424</v>
+      </c>
+      <c r="D37" s="1">
+        <f t="shared" si="2"/>
+        <v>7010.1028800000022</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>24</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="1">
         <f>B3</f>
         <v>159840</v>
       </c>
-      <c r="C38">
-        <f t="shared" si="0"/>
-        <v>18861.119999999995</v>
+      <c r="C38" s="1">
+        <f t="shared" si="0"/>
+        <v>5818.1759999999995</v>
+      </c>
+      <c r="D38" s="1">
+        <f t="shared" si="2"/>
+        <v>7000.9919999999993</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3">
-        <v>8000000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <f>K1*0.03</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8">
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9">
         <f>B3*B4*4</f>
-        <v>32000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10">
-        <f>B3*B5*B6*4</f>
-        <v>32000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <f>B3*B5*B6*4*4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <f>B3*B8</f>
-        <v>800000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="D14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1679,11 +1705,15 @@
         <v>20000</v>
       </c>
       <c r="C15" s="1">
-        <f>B15*4*(B$4+B$5*B$6)+B15*B$8+B15</f>
-        <v>22160</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <f>(B15*4/1000)*B$4+B15*B$5*B$6*16</f>
+        <v>728</v>
+      </c>
+      <c r="D15" s="1">
+        <f>(B16*4/1000)*B$4+B16*B$5*B$6*16*(0.9)+((B16)+B$8*B16)*0.1</f>
+        <v>4200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1692,115 +1722,151 @@
         <v>29411.764705882353</v>
       </c>
       <c r="C16" s="1">
-        <f>B16*4*(B$4+B$5*B$6)+B16*B$8+B16-B15</f>
-        <v>12588.235294117647</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ref="C16:C40" si="0">(B16*4/1000)*B$4+B16*B$5*B$6*16</f>
+        <v>1070.5882352941176</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" ref="D16:D18" si="1">(B16*4/1000)*B$4+B16*B$5*B$6*16*(0.9)+((B16-B15)+B$8*B16)*0.1</f>
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3</v>
       </c>
       <c r="B17" s="1">
-        <f t="shared" ref="B17:B24" si="0">1*(B26/17)</f>
+        <f t="shared" ref="B17:B24" si="2">1*(B26/17)</f>
         <v>44117.647058823532</v>
       </c>
       <c r="C17" s="1">
-        <f t="shared" ref="C17:C38" si="1">B17*4*(B$4+B$5*B$6)+B17*B$8+B17-B16</f>
-        <v>19470.588235294123</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>1605.8823529411766</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="1"/>
+        <v>3358.8235294117649</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>4</v>
       </c>
       <c r="B18" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>58823.529411764706</v>
       </c>
       <c r="C18" s="1">
-        <f t="shared" si="1"/>
-        <v>21058.823529411762</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2141.1764705882351</v>
+      </c>
+      <c r="D18" s="1">
+        <f>(B18*4/1000)*B$4+B18*B$5*B$6*16*(0.9)+((B18-B17)+B$8*B18)*0.1</f>
+        <v>3988.2352941176468</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>5</v>
       </c>
       <c r="B19" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>88235.294117647063</v>
       </c>
       <c r="C19" s="1">
-        <f t="shared" si="1"/>
-        <v>38941.176470588245</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>3211.7647058823532</v>
+      </c>
+      <c r="D19" s="1">
+        <f>(B19*4/1000)*B$4+B19*B$5*B$6*16*(0.9)+((B19-B18))*0.1</f>
+        <v>5835.2941176470595</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>6</v>
       </c>
       <c r="B20" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>111764.70588235294</v>
       </c>
       <c r="C20" s="1">
-        <f t="shared" si="1"/>
-        <v>35599.999999999985</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>4068.2352941176464</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" ref="D20:D40" si="3">(B20*4/1000)*B$4+B20*B$5*B$6*16*(0.9)+((B20-B19)+B$8*B20)*0.1</f>
+        <v>7136.4705882352937</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>7</v>
       </c>
       <c r="B21" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>141176.4705882353</v>
       </c>
       <c r="C21" s="1">
-        <f t="shared" si="1"/>
-        <v>44658.823529411791</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>5138.823529411764</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="3"/>
+        <v>8983.5294117647063</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>8</v>
       </c>
       <c r="B22" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>176470.58823529413</v>
       </c>
       <c r="C22" s="1">
-        <f t="shared" si="1"/>
-        <v>54352.941176470602</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>6423.5294117647063</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="3"/>
+        <v>11082.352941176472</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>9</v>
       </c>
       <c r="B23" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>205882.35294117648</v>
       </c>
       <c r="C23" s="1">
-        <f t="shared" si="1"/>
-        <v>51647.058823529427</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>7494.1176470588225</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="shared" si="3"/>
+        <v>11752.941176470587</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>10</v>
       </c>
       <c r="B24" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>235294.11764705883</v>
       </c>
       <c r="C24" s="1">
-        <f t="shared" si="1"/>
-        <v>54823.529411764699</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>8564.7058823529405</v>
+      </c>
+      <c r="D24" s="1">
+        <f t="shared" si="3"/>
+        <v>13011.764705882353</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>11</v>
       </c>
@@ -1808,143 +1874,191 @@
         <v>500000</v>
       </c>
       <c r="C25" s="1">
-        <f t="shared" si="1"/>
-        <v>318705.8823529412</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>18200</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" si="3"/>
+        <v>47870.588235294126</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>12</v>
       </c>
       <c r="B26">
         <v>750000</v>
       </c>
-      <c r="C26">
-        <f t="shared" si="1"/>
-        <v>331000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C26" s="1">
+        <f t="shared" si="0"/>
+        <v>27300</v>
+      </c>
+      <c r="D26" s="1">
+        <f t="shared" si="3"/>
+        <v>57100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>13</v>
       </c>
       <c r="B27">
         <v>1000000</v>
       </c>
-      <c r="C27">
-        <f t="shared" si="1"/>
-        <v>358000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C27" s="1">
+        <f t="shared" si="0"/>
+        <v>36400</v>
+      </c>
+      <c r="D27" s="1">
+        <f t="shared" si="3"/>
+        <v>67800</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>14</v>
       </c>
       <c r="B28">
         <v>1500000</v>
       </c>
-      <c r="C28">
-        <f t="shared" si="1"/>
-        <v>662000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="1">
+        <f t="shared" si="0"/>
+        <v>54600</v>
+      </c>
+      <c r="D28" s="1">
+        <f t="shared" si="3"/>
+        <v>114200</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>15</v>
       </c>
       <c r="B29">
         <v>1900000</v>
       </c>
-      <c r="C29">
-        <f t="shared" si="1"/>
-        <v>605200</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C29" s="1">
+        <f t="shared" si="0"/>
+        <v>69160</v>
+      </c>
+      <c r="D29" s="1">
+        <f t="shared" si="3"/>
+        <v>121320</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>16</v>
       </c>
       <c r="B30">
         <v>2400000</v>
       </c>
-      <c r="C30">
-        <f t="shared" si="1"/>
-        <v>759200</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C30" s="1">
+        <f t="shared" si="0"/>
+        <v>87360</v>
+      </c>
+      <c r="D30" s="1">
+        <f t="shared" si="3"/>
+        <v>152720</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>17</v>
       </c>
       <c r="B31">
         <v>3000000</v>
       </c>
-      <c r="C31">
-        <f t="shared" si="1"/>
-        <v>924000</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C31" s="1">
+        <f t="shared" si="0"/>
+        <v>109200</v>
+      </c>
+      <c r="D31" s="1">
+        <f t="shared" si="3"/>
+        <v>188400</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>18</v>
       </c>
       <c r="B32">
         <v>3500000</v>
       </c>
-      <c r="C32">
-        <f t="shared" si="1"/>
-        <v>878000</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C32" s="1">
+        <f t="shared" si="0"/>
+        <v>127400</v>
+      </c>
+      <c r="D32" s="1">
+        <f t="shared" si="3"/>
+        <v>199800</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>19</v>
       </c>
       <c r="B33">
         <v>4000000</v>
       </c>
-      <c r="C33">
-        <f t="shared" si="1"/>
-        <v>932000</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C33" s="1">
+        <f t="shared" si="0"/>
+        <v>145600</v>
+      </c>
+      <c r="D33" s="1">
+        <f t="shared" si="3"/>
+        <v>221200</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>20</v>
       </c>
       <c r="B34">
         <v>4500000</v>
       </c>
-      <c r="C34">
-        <f t="shared" si="1"/>
-        <v>986000</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C34" s="1">
+        <f t="shared" si="0"/>
+        <v>163800</v>
+      </c>
+      <c r="D34" s="1">
+        <f t="shared" si="3"/>
+        <v>242600</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>21</v>
       </c>
       <c r="B35">
         <v>5250000</v>
       </c>
-      <c r="C35">
-        <f t="shared" si="1"/>
-        <v>1317000</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C35" s="1">
+        <f t="shared" si="0"/>
+        <v>191100</v>
+      </c>
+      <c r="D35" s="1">
+        <f t="shared" si="3"/>
+        <v>299700</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>22</v>
       </c>
       <c r="B36">
         <v>6000000</v>
       </c>
-      <c r="C36">
-        <f t="shared" si="1"/>
-        <v>1398000</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C36" s="1">
+        <f t="shared" si="0"/>
+        <v>218400</v>
+      </c>
+      <c r="D36" s="1">
+        <f t="shared" si="3"/>
+        <v>331800</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>23</v>
       </c>
@@ -1952,21 +2066,55 @@
         <f>(B38+B36)/2</f>
         <v>6750000</v>
       </c>
-      <c r="C37">
-        <f t="shared" si="1"/>
-        <v>1479000</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C37" s="1">
+        <f t="shared" si="0"/>
+        <v>245700</v>
+      </c>
+      <c r="D37" s="1">
+        <f t="shared" si="3"/>
+        <v>363900</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>24</v>
       </c>
       <c r="B38">
         <v>7500000</v>
       </c>
-      <c r="C38">
-        <f t="shared" si="1"/>
-        <v>1560000</v>
+      <c r="C38" s="1">
+        <f t="shared" si="0"/>
+        <v>273000</v>
+      </c>
+      <c r="D38" s="1">
+        <f t="shared" si="3"/>
+        <v>396000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>30000000</v>
+      </c>
+      <c r="C39" s="1">
+        <f t="shared" si="0"/>
+        <v>1092000</v>
+      </c>
+      <c r="D39" s="1">
+        <f t="shared" si="3"/>
+        <v>3534000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>30000000</v>
+      </c>
+      <c r="C40" s="1">
+        <f t="shared" si="0"/>
+        <v>1092000</v>
+      </c>
+      <c r="D40" s="1">
+        <f t="shared" si="3"/>
+        <v>1284000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizando la presentacion de PxQ
</commit_message>
<xml_diff>
--- a/Assets/PxQVariosEscenarios.xlsx
+++ b/Assets/PxQVariosEscenarios.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>Escenario 1</t>
   </si>
@@ -73,6 +73,15 @@
   </si>
   <si>
     <t>Ganacia con costo descarga</t>
+  </si>
+  <si>
+    <t>Cantidad Usuarios (cientos)</t>
+  </si>
+  <si>
+    <t>Ganacia con costo descarga (USD)</t>
+  </si>
+  <si>
+    <t>Ganacia sin costo descarga (USD)</t>
   </si>
 </sst>
 </file>
@@ -355,11 +364,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="100814208"/>
-        <c:axId val="100852864"/>
+        <c:axId val="98255616"/>
+        <c:axId val="98257152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="100814208"/>
+        <c:axId val="98255616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -368,7 +377,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100852864"/>
+        <c:crossAx val="98257152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -376,7 +385,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100852864"/>
+        <c:axId val="98257152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -387,7 +396,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100814208"/>
+        <c:crossAx val="98255616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -433,96 +442,88 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Sheet2!$C$14</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Ganacia sin costo descarga</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Ganacia Versión no Paga (USD)</c:v>
           </c:tx>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$C$15:$C$38</c:f>
+              <c:f>Sheet1!$C$15:$C$38</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>728</c:v>
+                  <c:v>3.6399999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1070.5882352941176</c:v>
+                  <c:v>18.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1605.8823529411766</c:v>
+                  <c:v>36.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2141.1764705882351</c:v>
+                  <c:v>145.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3211.7647058823532</c:v>
+                  <c:v>364</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4068.2352941176464</c:v>
+                  <c:v>618.79999999999995</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5138.823529411764</c:v>
+                  <c:v>1092</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6423.5294117647063</c:v>
+                  <c:v>1820</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7494.1176470588225</c:v>
+                  <c:v>2548</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8564.7058823529405</c:v>
+                  <c:v>3567.2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>18200</c:v>
+                  <c:v>4280.6399999999994</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>27300</c:v>
+                  <c:v>4708.7039999999997</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>36400</c:v>
+                  <c:v>4755.7910400000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>54600</c:v>
+                  <c:v>4803.3489504000008</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>69160</c:v>
+                  <c:v>4827.3656951520006</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>87360</c:v>
+                  <c:v>5020.4603229580798</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>109200</c:v>
+                  <c:v>5171.0741326468233</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>127400</c:v>
+                  <c:v>5274.4956152997593</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>145600</c:v>
+                  <c:v>5432.7304837587526</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>163800</c:v>
+                  <c:v>5337.7175422771188</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>191100</c:v>
+                  <c:v>5560.1224398719996</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>218400</c:v>
+                  <c:v>5673.5943263999989</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>245700</c:v>
+                  <c:v>5759.99424</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>273000</c:v>
+                  <c:v>5818.1759999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -533,96 +534,180 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Sheet2!$D$14</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Ganacia con costo descarga</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Gancia Versión paga (USD)</c:v>
           </c:tx>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$D$15:$D$38</c:f>
+              <c:f>Sheet1!$D$15:$D$38</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>4200</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2200</c:v>
+                  <c:v>61.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3358.8235294117649</c:v>
+                  <c:v>92.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3988.2352941176468</c:v>
+                  <c:v>471.2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5835.2941176470595</c:v>
+                  <c:v>928</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7136.4705882352937</c:v>
+                  <c:v>1427.6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8983.5294117647063</c:v>
+                  <c:v>2584</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11082.352941176472</c:v>
+                  <c:v>4140</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11752.941176470587</c:v>
+                  <c:v>4996</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>13011.764705882353</c:v>
+                  <c:v>6994.4</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>47870.588235294126</c:v>
+                  <c:v>6993.28</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>57100</c:v>
+                  <c:v>6712.608000000002</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>67800</c:v>
+                  <c:v>5721.3340800000005</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>114200</c:v>
+                  <c:v>5778.5474208000023</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>121320</c:v>
+                  <c:v>5742.1133579039997</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>152720</c:v>
+                  <c:v>6433.6583682201599</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>188400</c:v>
+                  <c:v>6494.0481825867673</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>199800</c:v>
+                  <c:v>6486.0044120913008</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>221200</c:v>
+                  <c:v>6822.6470206256563</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>242600</c:v>
+                  <c:v>6015.1927654202582</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>299700</c:v>
+                  <c:v>7148.7288512640025</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>331800</c:v>
+                  <c:v>6982.8853247999987</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>363900</c:v>
+                  <c:v>7010.1028800000022</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>396000</c:v>
+                  <c:v>7000.9919999999993</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Cantidad Usuarios (cientos)</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$15:$E$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>980</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1176</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1293.6000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1306.5360000000003</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1319.6013600000003</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1326.1993668000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1379.247341472</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1420.6247617161603</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1449.0372569504834</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1492.508374658998</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1466.4059182079998</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1527.5061648000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1558.67976</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1582.4160000000002</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1598.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -639,11 +724,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="45958272"/>
-        <c:axId val="45959808"/>
+        <c:axId val="4606208"/>
+        <c:axId val="4616192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="45958272"/>
+        <c:axId val="4606208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -652,7 +737,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45959808"/>
+        <c:crossAx val="4616192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -660,7 +745,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="45959808"/>
+        <c:axId val="4616192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -671,7 +756,291 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45958272"/>
+        <c:crossAx val="4606208"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-AR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$C$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ganacia sin costo descarga (USD)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$C$15:$C$38</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>728</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1070.5882352941176</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1605.8823529411766</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2141.1764705882351</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3211.7647058823532</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4068.2352941176464</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5138.823529411764</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6423.5294117647063</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7494.1176470588225</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8564.7058823529405</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>18200</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>27300</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>36400</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>54600</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>69160</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>87360</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>109200</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>127400</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>145600</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>163800</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>191100</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>218400</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>245700</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>273000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$D$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ganacia con costo descarga (USD)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$D$15:$D$38</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>4200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3358.8235294117649</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3988.2352941176468</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5835.2941176470595</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7136.4705882352937</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8983.5294117647063</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11082.352941176472</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11752.941176470587</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13011.764705882353</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>47870.588235294126</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>57100</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>67800</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>114200</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>121320</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>152720</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>188400</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>199800</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>221200</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>242600</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>299700</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>331800</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>363900</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>396000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="102571008"/>
+        <c:axId val="102580992"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="102571008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="102580992"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="102580992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="102571008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -679,6 +1048,399 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-AR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$C$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ganacia sin costo descarga (USD)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$C$15:$C$38</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>728</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1070.5882352941176</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1605.8823529411766</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2141.1764705882351</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3211.7647058823532</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4068.2352941176464</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5138.823529411764</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6423.5294117647063</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7494.1176470588225</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8564.7058823529405</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>18200</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>27300</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>36400</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>54600</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>69160</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>87360</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>109200</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>127400</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>145600</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>163800</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>191100</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>218400</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>245700</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>273000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$D$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ganacia con costo descarga (USD)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$D$15:$D$38</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>4200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3358.8235294117649</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3988.2352941176468</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5835.2941176470595</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7136.4705882352937</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8983.5294117647063</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11082.352941176472</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11752.941176470587</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13011.764705882353</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>47870.588235294126</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>57100</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>67800</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>114200</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>121320</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>152720</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>188400</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>199800</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>221200</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>242600</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>299700</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>331800</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>363900</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>396000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$E$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cantidad Usuarios (cientos)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$E$15:$E$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>294.11764705882354</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>441.1764705882353</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>588.23529411764707</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>882.35294117647061</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1117.6470588235293</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1411.7647058823529</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1764.7058823529412</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2058.8235294117649</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2352.9411764705883</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7500</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>19000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>24000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>45000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>52500</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>67500</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>75000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="108799488"/>
+        <c:axId val="108801024"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="108799488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="108801024"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="108801024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="108799488"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="3.1027121609798768E-2"/>
+          <c:y val="0.72801509186351709"/>
+          <c:w val="0.93239020122484695"/>
+          <c:h val="0.24420713035870517"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -725,6 +1487,36 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -732,16 +1524,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>819150</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -755,6 +1547,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1052,13 +1874,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="A3:B11"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" customWidth="1"/>
     <col min="3" max="3" width="25.42578125" customWidth="1"/>
     <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1"/>
@@ -1192,6 +2014,10 @@
       <c r="D15" s="1">
         <v>4</v>
       </c>
+      <c r="E15">
+        <f>B15/100</f>
+        <v>1</v>
+      </c>
       <c r="G15">
         <f>30000/6</f>
         <v>5000</v>
@@ -1209,11 +2035,15 @@
         <v>18.2</v>
       </c>
       <c r="D16" s="1">
-        <f t="shared" ref="D15:D17" si="1">(B16*4/1000)*B$4+B16*B$5*B$6*16*(0.9)+((B16-B15)+B$8*B16)*0.1</f>
+        <f t="shared" ref="D16:D17" si="1">(B16*4/1000)*B$4+B16*B$5*B$6*16*(0.9)+((B16-B15)+B$8*B16)*0.1</f>
         <v>61.4</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <f t="shared" ref="E16:E38" si="2">B16/100</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3</v>
       </c>
@@ -1228,8 +2058,12 @@
         <f t="shared" si="1"/>
         <v>92.8</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>4</v>
       </c>
@@ -1244,8 +2078,12 @@
         <f>(B18*4/1000)*B$4+B18*B$5*B$6*16*(0.9)+((B18-B17)+B$8*B18)*0.1</f>
         <v>471.2</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>5</v>
       </c>
@@ -1260,8 +2098,12 @@
         <f>(B19*4/1000)*B$4+B19*B$5*B$6*16*(0.9)+((B19-B18))*0.1</f>
         <v>928</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>6</v>
       </c>
@@ -1273,11 +2115,15 @@
         <v>618.79999999999995</v>
       </c>
       <c r="D20" s="1">
-        <f t="shared" ref="D20:D38" si="2">(B20*4/1000)*B$4+B20*B$5*B$6*16*(0.9)+((B20-B19)+B$8*B20)*0.1</f>
+        <f t="shared" ref="D20:D38" si="3">(B20*4/1000)*B$4+B20*B$5*B$6*16*(0.9)+((B20-B19)+B$8*B20)*0.1</f>
         <v>1427.6</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <f t="shared" si="2"/>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>7</v>
       </c>
@@ -1289,11 +2135,15 @@
         <v>1092</v>
       </c>
       <c r="D21" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2584</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <f t="shared" si="2"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>8</v>
       </c>
@@ -1305,11 +2155,15 @@
         <v>1820</v>
       </c>
       <c r="D22" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4140</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <f t="shared" si="2"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>9</v>
       </c>
@@ -1321,11 +2175,15 @@
         <v>2548</v>
       </c>
       <c r="D23" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4996</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <f t="shared" si="2"/>
+        <v>700</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>10</v>
       </c>
@@ -1338,11 +2196,15 @@
         <v>3567.2</v>
       </c>
       <c r="D24" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6994.4</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <f t="shared" si="2"/>
+        <v>980</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>11</v>
       </c>
@@ -1355,11 +2217,15 @@
         <v>4280.6399999999994</v>
       </c>
       <c r="D25" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6993.28</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <f t="shared" si="2"/>
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>12</v>
       </c>
@@ -1372,11 +2238,15 @@
         <v>4708.7039999999997</v>
       </c>
       <c r="D26" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6712.608000000002</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <f t="shared" si="2"/>
+        <v>1293.6000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>13</v>
       </c>
@@ -1389,11 +2259,15 @@
         <v>4755.7910400000001</v>
       </c>
       <c r="D27" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5721.3340800000005</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <f t="shared" si="2"/>
+        <v>1306.5360000000003</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>14</v>
       </c>
@@ -1406,11 +2280,15 @@
         <v>4803.3489504000008</v>
       </c>
       <c r="D28" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5778.5474208000023</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <f t="shared" si="2"/>
+        <v>1319.6013600000003</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>15</v>
       </c>
@@ -1423,11 +2301,15 @@
         <v>4827.3656951520006</v>
       </c>
       <c r="D29" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5742.1133579039997</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <f t="shared" si="2"/>
+        <v>1326.1993668000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>16</v>
       </c>
@@ -1440,11 +2322,15 @@
         <v>5020.4603229580798</v>
       </c>
       <c r="D30" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6433.6583682201599</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30">
+        <f t="shared" si="2"/>
+        <v>1379.247341472</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>17</v>
       </c>
@@ -1457,11 +2343,15 @@
         <v>5171.0741326468233</v>
       </c>
       <c r="D31" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6494.0481825867673</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <f t="shared" si="2"/>
+        <v>1420.6247617161603</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>18</v>
       </c>
@@ -1474,11 +2364,15 @@
         <v>5274.4956152997593</v>
       </c>
       <c r="D32" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6486.0044120913008</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <f t="shared" si="2"/>
+        <v>1449.0372569504834</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>19</v>
       </c>
@@ -1491,11 +2385,15 @@
         <v>5432.7304837587526</v>
       </c>
       <c r="D33" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6822.6470206256563</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <f t="shared" si="2"/>
+        <v>1492.508374658998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>20</v>
       </c>
@@ -1508,11 +2406,15 @@
         <v>5337.7175422771188</v>
       </c>
       <c r="D34" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6015.1927654202582</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <f t="shared" si="2"/>
+        <v>1466.4059182079998</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>21</v>
       </c>
@@ -1525,11 +2427,15 @@
         <v>5560.1224398719996</v>
       </c>
       <c r="D35" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7148.7288512640025</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35">
+        <f t="shared" si="2"/>
+        <v>1527.5061648000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>22</v>
       </c>
@@ -1542,11 +2448,15 @@
         <v>5673.5943263999989</v>
       </c>
       <c r="D36" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6982.8853247999987</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <f t="shared" si="2"/>
+        <v>1558.67976</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>23</v>
       </c>
@@ -1559,11 +2469,15 @@
         <v>5759.99424</v>
       </c>
       <c r="D37" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7010.1028800000022</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37">
+        <f t="shared" si="2"/>
+        <v>1582.4160000000002</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>24</v>
       </c>
@@ -1576,8 +2490,12 @@
         <v>5818.1759999999995</v>
       </c>
       <c r="D38" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7000.9919999999993</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="2"/>
+        <v>1598.4</v>
       </c>
     </row>
   </sheetData>
@@ -1589,10 +2507,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="C17" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32:E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1606,7 +2524,7 @@
     <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1614,7 +2532,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1623,7 +2541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1631,7 +2549,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1639,7 +2557,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1647,8 +2565,8 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1656,7 +2574,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1665,7 +2583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1674,7 +2592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1683,7 +2601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1691,13 +2609,16 @@
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="E14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1712,8 +2633,12 @@
         <f>(B16*4/1000)*B$4+B16*B$5*B$6*16*(0.9)+((B16)+B$8*B16)*0.1</f>
         <v>4200</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <f>B15/100</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1726,16 +2651,20 @@
         <v>1070.5882352941176</v>
       </c>
       <c r="D16" s="1">
-        <f t="shared" ref="D16:D18" si="1">(B16*4/1000)*B$4+B16*B$5*B$6*16*(0.9)+((B16-B15)+B$8*B16)*0.1</f>
+        <f t="shared" ref="D16:D17" si="1">(B16*4/1000)*B$4+B16*B$5*B$6*16*(0.9)+((B16-B15)+B$8*B16)*0.1</f>
         <v>2200</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <f t="shared" ref="E16:E40" si="2">B16/100</f>
+        <v>294.11764705882354</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3</v>
       </c>
       <c r="B17" s="1">
-        <f t="shared" ref="B17:B24" si="2">1*(B26/17)</f>
+        <f t="shared" ref="B17:B24" si="3">1*(B26/17)</f>
         <v>44117.647058823532</v>
       </c>
       <c r="C17" s="1">
@@ -1746,13 +2675,17 @@
         <f t="shared" si="1"/>
         <v>3358.8235294117649</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <f t="shared" si="2"/>
+        <v>441.1764705882353</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>4</v>
       </c>
       <c r="B18" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>58823.529411764706</v>
       </c>
       <c r="C18" s="1">
@@ -1763,13 +2696,17 @@
         <f>(B18*4/1000)*B$4+B18*B$5*B$6*16*(0.9)+((B18-B17)+B$8*B18)*0.1</f>
         <v>3988.2352941176468</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <f t="shared" si="2"/>
+        <v>588.23529411764707</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>5</v>
       </c>
       <c r="B19" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>88235.294117647063</v>
       </c>
       <c r="C19" s="1">
@@ -1780,13 +2717,17 @@
         <f>(B19*4/1000)*B$4+B19*B$5*B$6*16*(0.9)+((B19-B18))*0.1</f>
         <v>5835.2941176470595</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <f t="shared" si="2"/>
+        <v>882.35294117647061</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>6</v>
       </c>
       <c r="B20" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>111764.70588235294</v>
       </c>
       <c r="C20" s="1">
@@ -1794,16 +2735,20 @@
         <v>4068.2352941176464</v>
       </c>
       <c r="D20" s="1">
-        <f t="shared" ref="D20:D40" si="3">(B20*4/1000)*B$4+B20*B$5*B$6*16*(0.9)+((B20-B19)+B$8*B20)*0.1</f>
+        <f t="shared" ref="D20:D40" si="4">(B20*4/1000)*B$4+B20*B$5*B$6*16*(0.9)+((B20-B19)+B$8*B20)*0.1</f>
         <v>7136.4705882352937</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <f t="shared" si="2"/>
+        <v>1117.6470588235293</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>7</v>
       </c>
       <c r="B21" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>141176.4705882353</v>
       </c>
       <c r="C21" s="1">
@@ -1811,16 +2756,20 @@
         <v>5138.823529411764</v>
       </c>
       <c r="D21" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8983.5294117647063</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <f t="shared" si="2"/>
+        <v>1411.7647058823529</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>8</v>
       </c>
       <c r="B22" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>176470.58823529413</v>
       </c>
       <c r="C22" s="1">
@@ -1828,16 +2777,20 @@
         <v>6423.5294117647063</v>
       </c>
       <c r="D22" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>11082.352941176472</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <f t="shared" si="2"/>
+        <v>1764.7058823529412</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>9</v>
       </c>
       <c r="B23" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>205882.35294117648</v>
       </c>
       <c r="C23" s="1">
@@ -1845,16 +2798,20 @@
         <v>7494.1176470588225</v>
       </c>
       <c r="D23" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>11752.941176470587</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <f t="shared" si="2"/>
+        <v>2058.8235294117649</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>10</v>
       </c>
       <c r="B24" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>235294.11764705883</v>
       </c>
       <c r="C24" s="1">
@@ -1862,11 +2819,15 @@
         <v>8564.7058823529405</v>
       </c>
       <c r="D24" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>13011.764705882353</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <f t="shared" si="2"/>
+        <v>2352.9411764705883</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>11</v>
       </c>
@@ -1878,11 +2839,15 @@
         <v>18200</v>
       </c>
       <c r="D25" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>47870.588235294126</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <f t="shared" si="2"/>
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>12</v>
       </c>
@@ -1894,11 +2859,15 @@
         <v>27300</v>
       </c>
       <c r="D26" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>57100</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <f t="shared" si="2"/>
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>13</v>
       </c>
@@ -1910,11 +2879,15 @@
         <v>36400</v>
       </c>
       <c r="D27" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>67800</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <f t="shared" si="2"/>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>14</v>
       </c>
@@ -1926,11 +2899,15 @@
         <v>54600</v>
       </c>
       <c r="D28" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>114200</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <f t="shared" si="2"/>
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>15</v>
       </c>
@@ -1942,11 +2919,15 @@
         <v>69160</v>
       </c>
       <c r="D29" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>121320</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <f t="shared" si="2"/>
+        <v>19000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>16</v>
       </c>
@@ -1958,11 +2939,15 @@
         <v>87360</v>
       </c>
       <c r="D30" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>152720</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30">
+        <f t="shared" si="2"/>
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>17</v>
       </c>
@@ -1974,11 +2959,15 @@
         <v>109200</v>
       </c>
       <c r="D31" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>188400</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <f t="shared" si="2"/>
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>18</v>
       </c>
@@ -1990,11 +2979,15 @@
         <v>127400</v>
       </c>
       <c r="D32" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>199800</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <f t="shared" si="2"/>
+        <v>35000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>19</v>
       </c>
@@ -2006,11 +2999,15 @@
         <v>145600</v>
       </c>
       <c r="D33" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>221200</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <f t="shared" si="2"/>
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>20</v>
       </c>
@@ -2022,11 +3019,15 @@
         <v>163800</v>
       </c>
       <c r="D34" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>242600</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <f t="shared" si="2"/>
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>21</v>
       </c>
@@ -2038,11 +3039,15 @@
         <v>191100</v>
       </c>
       <c r="D35" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>299700</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35">
+        <f t="shared" si="2"/>
+        <v>52500</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>22</v>
       </c>
@@ -2054,11 +3059,15 @@
         <v>218400</v>
       </c>
       <c r="D36" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>331800</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <f t="shared" si="2"/>
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>23</v>
       </c>
@@ -2071,11 +3080,15 @@
         <v>245700</v>
       </c>
       <c r="D37" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>363900</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37">
+        <f t="shared" si="2"/>
+        <v>67500</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>24</v>
       </c>
@@ -2087,11 +3100,15 @@
         <v>273000</v>
       </c>
       <c r="D38" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>396000</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38">
+        <f t="shared" si="2"/>
+        <v>75000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>30000000</v>
       </c>
@@ -2100,11 +3117,15 @@
         <v>1092000</v>
       </c>
       <c r="D39" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3534000</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39">
+        <f t="shared" si="2"/>
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>30000000</v>
       </c>
@@ -2113,8 +3134,12 @@
         <v>1092000</v>
       </c>
       <c r="D40" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1284000</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="2"/>
+        <v>300000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>